<commit_message>
added code to identify SLA records only available in TRY
</commit_message>
<xml_diff>
--- a/data/traits/alterations to RG dataset.xlsx
+++ b/data/traits/alterations to RG dataset.xlsx
@@ -9,12 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="SLA" sheetId="1" r:id="rId1"/>
-    <sheet name="suspicious data" sheetId="3" r:id="rId2"/>
-    <sheet name="readme" sheetId="2" r:id="rId3"/>
+    <sheet name="readme" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="76">
   <si>
     <t>Species</t>
   </si>
@@ -58,12 +57,6 @@
     <t>Smilax australis</t>
   </si>
   <si>
-    <t>cm2/g</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Gallagher_field_workPHD</t>
   </si>
   <si>
@@ -235,9 +228,6 @@
     <t>Passiflora edulis</t>
   </si>
   <si>
-    <t>AUSTRAITS_dataset_32</t>
-  </si>
-  <si>
     <t>cm2/g &gt; m2/kg</t>
   </si>
   <si>
@@ -263,24 +253,6 @@
   </si>
   <si>
     <t>m2/kg &gt; cm2/g</t>
-  </si>
-  <si>
-    <t>Taxon</t>
-  </si>
-  <si>
-    <t>SLA</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>SLA.units</t>
-  </si>
-  <si>
-    <t>SLAfromLMA</t>
-  </si>
-  <si>
-    <t>Lawson_field_work</t>
   </si>
 </sst>
 </file>
@@ -296,7 +268,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -306,12 +278,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -328,10 +294,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C215"/>
   <sheetViews>
-    <sheetView topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="K216" sqref="K216"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,7 +609,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -655,7 +620,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -666,546 +631,546 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C32" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C33" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C34" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C35" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C36" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B37" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C37" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B38" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C38" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C39" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C40" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B41" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C41" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B42" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C42" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B43" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C43" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B44" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C44" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B45" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B46" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C46" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B47" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C47" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B48" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C48" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B49" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C49" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B50" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C50" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B51" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C51" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B52" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C52" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B53" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C53" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B54" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C54" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B55" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C55" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B56" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C56" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1213,120 +1178,120 @@
         <v>9</v>
       </c>
       <c r="B57" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C57" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B58" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C58" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B59" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C59" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C60" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B61" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C61" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B62" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C62" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B63" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C63" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B64" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C64" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B65" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C65" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B66" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C66" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B67" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C67" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1334,208 +1299,208 @@
         <v>5</v>
       </c>
       <c r="B68" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C68" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B69" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C69" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B70" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C70" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B71" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C71" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B72" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C72" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B73" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C73" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B74" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C74" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B75" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C75" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B76" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C76" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B77" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C77" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B78" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C78" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B79" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C79" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B80" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C80" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B81" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C81" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B82" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C82" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B83" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C83" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B84" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C84" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B85" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C85" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B86" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C86" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -1543,10 +1508,10 @@
         <v>5</v>
       </c>
       <c r="B87" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C87" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -1554,21 +1519,21 @@
         <v>9</v>
       </c>
       <c r="B88" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C88" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B89" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C89" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -1576,98 +1541,98 @@
         <v>9</v>
       </c>
       <c r="B90" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C90" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B91" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C91" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B92" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C92" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B93" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C93" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B94" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C94" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B95" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C95" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B96" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C96" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B97" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C97" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B98" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C98" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -1675,395 +1640,395 @@
         <v>9</v>
       </c>
       <c r="B100" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C100" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B101" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C101" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B102" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C102" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B103" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C103" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B104" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C104" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B105" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C105" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B106" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C106" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B107" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C107" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B108" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C108" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B109" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C109" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B110" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C110" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B111" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C111" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B112" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C112" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B113" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C113" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B114" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C114" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B115" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C115" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B117" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C117" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B118" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C118" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B119" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C119" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B120" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C120" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B121" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C121" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B122" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C122" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B123" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C123" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B124" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C124" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B125" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C125" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B126" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C126" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B127" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C127" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B128" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C128" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B129" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C129" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B130" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C130" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B131" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C131" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B132" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C132" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B133" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C133" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B134" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C134" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B135" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C135" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B136" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C136" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -2071,857 +2036,857 @@
         <v>9</v>
       </c>
       <c r="B137" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C137" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B138" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C138" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B139" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C139" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B140" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C140" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B141" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C141" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B142" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C142" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B143" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C143" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B144" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C144" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B145" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C145" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B146" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C146" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B147" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C147" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B148" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C148" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B149" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C149" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B150" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C150" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B151" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C151" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B152" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C152" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B153" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C153" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B154" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C154" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B155" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C155" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B156" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C156" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B157" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C157" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B158" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C158" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B159" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C159" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B160" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C160" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B161" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C161" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B162" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C162" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B163" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C163" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B164" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C164" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B165" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C165" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B166" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C166" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B167" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C167" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B168" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C168" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B169" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C169" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B170" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C170" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B171" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C171" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B172" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C172" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B173" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C173" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B174" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C174" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B175" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C175" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B176" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C176" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B177" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C177" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B178" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C178" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B179" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C179" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B180" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C180" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B181" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C181" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B182" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C182" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B183" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C183" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B184" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C184" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B185" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C185" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B186" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C186" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B187" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C187" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B188" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C188" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B189" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C189" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B190" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C190" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B191" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C191" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B192" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C192" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B193" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C193" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B194" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C194" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B195" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C195" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B196" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C196" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B197" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C197" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B198" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C198" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B199" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C199" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B200" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C200" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B201" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C201" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B202" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C202" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B203" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C203" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B204" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C204" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B205" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C205" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B206" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C206" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B207" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C207" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B208" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C208" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B209" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C209" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B210" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C210" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B211" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C211" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B212" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C212" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B213" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C213" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B215" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C215" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2931,225 +2896,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2">
-        <v>5.56</v>
-      </c>
-      <c r="C2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3">
-        <v>4.1990999999999996</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4">
-        <v>5.3575999999999997</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1.6559999999999999</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="2">
-        <v>3.3769999999999998</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="2">
-        <v>2.4769999999999999</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="2">
-        <v>6.431</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1.8240000000000001</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="2">
-        <v>7.0069999999999997</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11">
-        <v>12.893373609999999</v>
-      </c>
-      <c r="C11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState ref="A2:F11">
-    <sortCondition ref="E2:E11"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
added code to find dodgy leaf area data
</commit_message>
<xml_diff>
--- a/data/traits/alterations to RG dataset.xlsx
+++ b/data/traits/alterations to RG dataset.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SLA" sheetId="1" r:id="rId1"/>
-    <sheet name="readme" sheetId="2" r:id="rId2"/>
+    <sheet name="dodgy leaf areas" sheetId="4" r:id="rId2"/>
+    <sheet name="readme" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="95">
   <si>
     <t>Species</t>
   </si>
@@ -253,14 +254,79 @@
   </si>
   <si>
     <t>m2/kg &gt; cm2/g</t>
+  </si>
+  <si>
+    <t>AUSTRAITS_dataset_68</t>
+  </si>
+  <si>
+    <t>Araucaria cunninghamii</t>
+  </si>
+  <si>
+    <t>AUSTRAITS_dataset_49</t>
+  </si>
+  <si>
+    <t>Carissa ovata</t>
+  </si>
+  <si>
+    <t>AUSTRAITS_dataset_6</t>
+  </si>
+  <si>
+    <t>AUSTRAITS_dataset_32</t>
+  </si>
+  <si>
+    <t>AUSTRAITS_dataset_29</t>
+  </si>
+  <si>
+    <t>Melodinus australis</t>
+  </si>
+  <si>
+    <t>Melodorum leichhardtii</t>
+  </si>
+  <si>
+    <t>Polyscias elegans</t>
+  </si>
+  <si>
+    <t>AUSTRAITS_dataset_61</t>
+  </si>
+  <si>
+    <t>AUSTRAITS_dataset_43</t>
+  </si>
+  <si>
+    <t>Rubus moluccanus</t>
+  </si>
+  <si>
+    <t>AUSTRAITS_dataset_12</t>
+  </si>
+  <si>
+    <t>AUSTRAITS_dataset_28</t>
+  </si>
+  <si>
+    <t>AUSTRAITS_dataset_3</t>
+  </si>
+  <si>
+    <t>SPECIES</t>
+  </si>
+  <si>
+    <t>VALUE</t>
+  </si>
+  <si>
+    <t>SOURCE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -294,9 +360,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,7 +646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C215"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
@@ -2896,6 +2963,1169 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C120"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2">
+        <v>0.4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4">
+        <v>0.219</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5">
+        <v>0.75</v>
+      </c>
+      <c r="C5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>21.95</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>47.25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>90.56</v>
+      </c>
+      <c r="C9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>546.75</v>
+      </c>
+      <c r="C10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12">
+        <v>3.75</v>
+      </c>
+      <c r="C12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13">
+        <v>4.62</v>
+      </c>
+      <c r="C13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14">
+        <v>46.2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16">
+        <v>27.65</v>
+      </c>
+      <c r="C16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17">
+        <v>29.332999999999998</v>
+      </c>
+      <c r="C17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18">
+        <v>30.625</v>
+      </c>
+      <c r="C18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19">
+        <v>483.9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20">
+        <v>27.651</v>
+      </c>
+      <c r="C20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22">
+        <v>1E-3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23">
+        <v>1.9E-2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24">
+        <v>0.188</v>
+      </c>
+      <c r="C24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <v>0.19</v>
+      </c>
+      <c r="C25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27">
+        <v>0.9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29">
+        <v>61.33</v>
+      </c>
+      <c r="C29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>1.5389999999999999</v>
+      </c>
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>8.1579999999999995</v>
+      </c>
+      <c r="C31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>15.39</v>
+      </c>
+      <c r="C32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33">
+        <v>19.54</v>
+      </c>
+      <c r="C33" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34">
+        <v>19.541</v>
+      </c>
+      <c r="C34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35">
+        <v>23.385000000000002</v>
+      </c>
+      <c r="C35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36">
+        <v>23.39</v>
+      </c>
+      <c r="C36" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37">
+        <v>28.125</v>
+      </c>
+      <c r="C37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38">
+        <v>28.13</v>
+      </c>
+      <c r="C38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39">
+        <v>81.58</v>
+      </c>
+      <c r="C39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40">
+        <v>83.808999999999997</v>
+      </c>
+      <c r="C40" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41">
+        <v>83.81</v>
+      </c>
+      <c r="C41" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43">
+        <v>10.5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44">
+        <v>24.82</v>
+      </c>
+      <c r="C44" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45">
+        <v>49.613</v>
+      </c>
+      <c r="C45" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46">
+        <v>110.25</v>
+      </c>
+      <c r="C46" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48">
+        <v>21</v>
+      </c>
+      <c r="C48" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49">
+        <v>22.05</v>
+      </c>
+      <c r="C49" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>84</v>
+      </c>
+      <c r="B50">
+        <v>37.19</v>
+      </c>
+      <c r="C50" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>84</v>
+      </c>
+      <c r="B51">
+        <v>396.9</v>
+      </c>
+      <c r="C51" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>20</v>
+      </c>
+      <c r="B53">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="C53" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>20</v>
+      </c>
+      <c r="B54">
+        <v>2.1819999999999999</v>
+      </c>
+      <c r="C54" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>20</v>
+      </c>
+      <c r="B55">
+        <v>5.2</v>
+      </c>
+      <c r="C55" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>20</v>
+      </c>
+      <c r="B56">
+        <v>5.6</v>
+      </c>
+      <c r="C56" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>20</v>
+      </c>
+      <c r="B57">
+        <v>5.6859999999999999</v>
+      </c>
+      <c r="C57" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>20</v>
+      </c>
+      <c r="B58">
+        <v>6.55</v>
+      </c>
+      <c r="C58" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>20</v>
+      </c>
+      <c r="B59">
+        <v>13.93</v>
+      </c>
+      <c r="C59" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>20</v>
+      </c>
+      <c r="B60">
+        <v>14.02</v>
+      </c>
+      <c r="C60" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>20</v>
+      </c>
+      <c r="B61">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="C61" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>20</v>
+      </c>
+      <c r="B62">
+        <v>26.25</v>
+      </c>
+      <c r="C62" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>19</v>
+      </c>
+      <c r="B64">
+        <v>5.1260000000000003</v>
+      </c>
+      <c r="C64" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>19</v>
+      </c>
+      <c r="B65">
+        <v>5.13</v>
+      </c>
+      <c r="C65" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>19</v>
+      </c>
+      <c r="B66">
+        <v>6.83</v>
+      </c>
+      <c r="C66" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>19</v>
+      </c>
+      <c r="B67">
+        <v>16.059999999999999</v>
+      </c>
+      <c r="C67" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>19</v>
+      </c>
+      <c r="B68">
+        <v>50.03</v>
+      </c>
+      <c r="C68" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>19</v>
+      </c>
+      <c r="B69">
+        <v>25.3</v>
+      </c>
+      <c r="C69" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>19</v>
+      </c>
+      <c r="B70">
+        <v>26.98</v>
+      </c>
+      <c r="C70" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>19</v>
+      </c>
+      <c r="B71">
+        <v>31.53</v>
+      </c>
+      <c r="C71" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>19</v>
+      </c>
+      <c r="B72">
+        <v>43.51</v>
+      </c>
+      <c r="C72" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>19</v>
+      </c>
+      <c r="B73">
+        <v>44.33</v>
+      </c>
+      <c r="C73" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>19</v>
+      </c>
+      <c r="B74">
+        <v>49</v>
+      </c>
+      <c r="C74" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>19</v>
+      </c>
+      <c r="B75">
+        <v>54.24</v>
+      </c>
+      <c r="C75" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>85</v>
+      </c>
+      <c r="B77">
+        <v>16.98</v>
+      </c>
+      <c r="C77" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>85</v>
+      </c>
+      <c r="B78">
+        <v>26.917000000000002</v>
+      </c>
+      <c r="C78" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>85</v>
+      </c>
+      <c r="B79">
+        <v>27.36</v>
+      </c>
+      <c r="C79" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>85</v>
+      </c>
+      <c r="B80">
+        <v>28.35</v>
+      </c>
+      <c r="C80" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>85</v>
+      </c>
+      <c r="B81">
+        <v>32.97</v>
+      </c>
+      <c r="C81" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>85</v>
+      </c>
+      <c r="B82">
+        <v>33.380000000000003</v>
+      </c>
+      <c r="C82" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>85</v>
+      </c>
+      <c r="B83">
+        <v>35.9</v>
+      </c>
+      <c r="C83" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>85</v>
+      </c>
+      <c r="B84">
+        <v>323.36</v>
+      </c>
+      <c r="C84" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>88</v>
+      </c>
+      <c r="B86">
+        <v>38.68</v>
+      </c>
+      <c r="C86" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>88</v>
+      </c>
+      <c r="B87">
+        <v>64.313000000000002</v>
+      </c>
+      <c r="C87" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>88</v>
+      </c>
+      <c r="B88">
+        <v>324.8</v>
+      </c>
+      <c r="C88" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>16</v>
+      </c>
+      <c r="B91">
+        <v>2.72</v>
+      </c>
+      <c r="C91" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>16</v>
+      </c>
+      <c r="B92">
+        <v>3.6840000000000002</v>
+      </c>
+      <c r="C92" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>16</v>
+      </c>
+      <c r="B93">
+        <v>4.4279999999999999</v>
+      </c>
+      <c r="C93" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>16</v>
+      </c>
+      <c r="B94">
+        <v>19.553000000000001</v>
+      </c>
+      <c r="C94" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>26</v>
+      </c>
+      <c r="B96">
+        <v>10.097</v>
+      </c>
+      <c r="C96" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>26</v>
+      </c>
+      <c r="B97">
+        <v>8.6460000000000008</v>
+      </c>
+      <c r="C97" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>26</v>
+      </c>
+      <c r="B98">
+        <v>8.9909999999999997</v>
+      </c>
+      <c r="C98" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>26</v>
+      </c>
+      <c r="B99">
+        <v>14.798</v>
+      </c>
+      <c r="C99" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>26</v>
+      </c>
+      <c r="B100">
+        <v>19.004000000000001</v>
+      </c>
+      <c r="C100" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>26</v>
+      </c>
+      <c r="B101">
+        <v>10.456</v>
+      </c>
+      <c r="C101" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>26</v>
+      </c>
+      <c r="B102">
+        <v>10.5</v>
+      </c>
+      <c r="C102" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>26</v>
+      </c>
+      <c r="B103">
+        <v>11.21</v>
+      </c>
+      <c r="C103" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>26</v>
+      </c>
+      <c r="B104">
+        <v>13.183</v>
+      </c>
+      <c r="C104" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>26</v>
+      </c>
+      <c r="B105">
+        <v>16.21</v>
+      </c>
+      <c r="C105" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>26</v>
+      </c>
+      <c r="B106">
+        <v>16.920000000000002</v>
+      </c>
+      <c r="C106" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>26</v>
+      </c>
+      <c r="B107">
+        <v>18.375</v>
+      </c>
+      <c r="C107" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>26</v>
+      </c>
+      <c r="B108">
+        <v>18.670999999999999</v>
+      </c>
+      <c r="C108" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>26</v>
+      </c>
+      <c r="B109">
+        <v>18.72</v>
+      </c>
+      <c r="C109" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>26</v>
+      </c>
+      <c r="B110">
+        <v>25.1</v>
+      </c>
+      <c r="C110" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>26</v>
+      </c>
+      <c r="B111">
+        <v>24.16</v>
+      </c>
+      <c r="C111" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>26</v>
+      </c>
+      <c r="B112">
+        <v>24.427</v>
+      </c>
+      <c r="C112" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>26</v>
+      </c>
+      <c r="B113">
+        <v>28.695</v>
+      </c>
+      <c r="C113" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>26</v>
+      </c>
+      <c r="B114">
+        <v>0.104</v>
+      </c>
+      <c r="C114" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>26</v>
+      </c>
+      <c r="B115">
+        <v>29.64</v>
+      </c>
+      <c r="C115" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>26</v>
+      </c>
+      <c r="B116">
+        <v>33.28</v>
+      </c>
+      <c r="C116" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>26</v>
+      </c>
+      <c r="B117">
+        <v>107.663</v>
+      </c>
+      <c r="C117" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>26</v>
+      </c>
+      <c r="B118">
+        <v>187.71799999999999</v>
+      </c>
+      <c r="C118" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>26</v>
+      </c>
+      <c r="B119">
+        <v>203.55699999999999</v>
+      </c>
+      <c r="C119" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>26</v>
+      </c>
+      <c r="B120">
+        <v>203.56</v>
+      </c>
+      <c r="C120" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>